<commit_message>
bug sur repetition equipe sur un seul jour
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_B.xlsx
+++ b/matrice_temps/horaire_B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Equipes</t>
   </si>
@@ -28,7 +28,61 @@
     <t>C. Ronaldo</t>
   </si>
   <si>
-    <t>Semaine 6</t>
+    <t>L. Messi</t>
+  </si>
+  <si>
+    <t>K. Bryant</t>
+  </si>
+  <si>
+    <t>R. Federer</t>
+  </si>
+  <si>
+    <t>P. Mickelson</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>R. Nadal</t>
+  </si>
+  <si>
+    <t>M. Ryan</t>
+  </si>
+  <si>
+    <t>M. Pacquiao</t>
+  </si>
+  <si>
+    <t>Z. Ibrahimović</t>
+  </si>
+  <si>
+    <t>D. Rose</t>
+  </si>
+  <si>
+    <t>G. Bale</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>R. Falcao</t>
+  </si>
+  <si>
+    <t>M. Özil</t>
+  </si>
+  <si>
+    <t>N. Djokovic</t>
+  </si>
+  <si>
+    <t>M. Stafford</t>
+  </si>
+  <si>
+    <t>L. Hamilton</t>
+  </si>
+  <si>
+    <t>K. Durant</t>
+  </si>
+  <si>
+    <t>Semaine 13</t>
   </si>
   <si>
     <t>Horaire</t>
@@ -69,6 +123,18 @@
   <si>
     <t>dimanche
 2022-04-03</t>
+  </si>
+  <si>
+    <t>A B</t>
+  </si>
+  <si>
+    <t>C A</t>
+  </si>
+  <si>
+    <t>B C</t>
+  </si>
+  <si>
+    <t>Modele : repartition concentre h-pers = 900</t>
   </si>
 </sst>
 </file>
@@ -420,14 +486,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="15.7109375" customWidth="1"/>
-    <col min="2" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="10" width="15.7109375" customWidth="1"/>
+    <col min="2" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -437,73 +503,164 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="2" t="s">
-        <v>12</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Encore bug repart. eq par jour
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_B.xlsx
+++ b/matrice_temps/horaire_B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Equipes</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>A B</t>
-  </si>
-  <si>
-    <t>C A</t>
   </si>
   <si>
     <t>B C</t>
@@ -601,7 +598,7 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -609,7 +606,7 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -620,10 +617,10 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
         <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -634,7 +631,7 @@
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -642,25 +639,37 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:2">
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="2:2">
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nouveau modele + nouveau bug
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_B.xlsx
+++ b/matrice_temps/horaire_B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Equipes</t>
   </si>
@@ -28,7 +28,70 @@
     <t>C. Ronaldo</t>
   </si>
   <si>
-    <t>Semaine 1</t>
+    <t>L. James</t>
+  </si>
+  <si>
+    <t>L. Messi</t>
+  </si>
+  <si>
+    <t>K. Bryant</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>T. Woods</t>
+  </si>
+  <si>
+    <t>R. Federer</t>
+  </si>
+  <si>
+    <t>P. Mickelson</t>
+  </si>
+  <si>
+    <t>R. Nadal</t>
+  </si>
+  <si>
+    <t>M. Ryan</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>M. Pacquiao</t>
+  </si>
+  <si>
+    <t>Z. Ibrahimović</t>
+  </si>
+  <si>
+    <t>D. Rose</t>
+  </si>
+  <si>
+    <t>G. Bale</t>
+  </si>
+  <si>
+    <t>R. Falcao</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>M. Özil</t>
+  </si>
+  <si>
+    <t>N. Djokovic</t>
+  </si>
+  <si>
+    <t>M. Stafford</t>
+  </si>
+  <si>
+    <t>L. Hamilton</t>
+  </si>
+  <si>
+    <t>K. Durant</t>
+  </si>
+  <si>
+    <t>Semaine 14</t>
   </si>
   <si>
     <t>Horaire</t>
@@ -44,46 +107,55 @@
   </si>
   <si>
     <t>Lundi
-2022-01-03</t>
+2022-04-04</t>
   </si>
   <si>
     <t>Mardi
-2022-01-04</t>
+2022-04-05</t>
   </si>
   <si>
     <t>Mercredi
-2022-01-05</t>
+2022-04-06</t>
   </si>
   <si>
     <t>Jeudi
-2022-01-06</t>
+2022-04-07</t>
   </si>
   <si>
     <t>Vendredi
-2022-01-07</t>
+2022-04-08</t>
   </si>
   <si>
     <t>Samedi
-2022-01-08</t>
+2022-04-09</t>
   </si>
   <si>
     <t>dimanche
-2022-01-09</t>
-  </si>
-  <si>
-    <t>Modele : repartition_etendu h-pers = 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> date de réf. :2022-01-07 12:12:00 
- sem : 1
- Modele : repartition_etendu h-pers = 40
- Calcul présences totales d'équipes: 3
- Calcul présences individuelles: 6.7
- Créneaux par jour: 1
- Equipes par créneau: 1
- Nombre d'équipes: 1
- Empl. par éq.: 2
- Durée quart.: 6.0
+2022-04-10</t>
+  </si>
+  <si>
+    <t>A B</t>
+  </si>
+  <si>
+    <t>C D</t>
+  </si>
+  <si>
+    <t>B C</t>
+  </si>
+  <si>
+    <t>Modele : repartition concentre h-pers = 1050</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> date de réf. :2022-04-08 12:12:00 
+ sem : 14
+ Modele : repartition concentre h-pers = 1050
+ Calcul présences totales d'équipes: 30
+ Calcul présences individuelles: 150.0
+ Créneaux par jour: 3
+ Equipes par créneau: 2
+ Nombre d'équipes: 4
+ Empl. par éq.: 5
+ Durée quart.: 7.0
 </t>
   </si>
 </sst>
@@ -436,14 +508,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="17" width="20.7109375" customWidth="1"/>
-    <col min="2" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="20" width="20.7109375" customWidth="1"/>
+    <col min="2" max="16" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -453,86 +525,182 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="2" t="s">
-        <v>11</v>
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorg pour affectations dans equipes a la fin
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_B.xlsx
+++ b/matrice_temps/horaire_B.xlsx
@@ -14,148 +14,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Equipes</t>
   </si>
   <si>
+    <t>Semaine 13</t>
+  </si>
+  <si>
+    <t>Horaire</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Lundi
+2022-03-28</t>
+  </si>
+  <si>
+    <t>Mardi
+2022-03-29</t>
+  </si>
+  <si>
+    <t>Mercredi
+2022-03-30</t>
+  </si>
+  <si>
+    <t>Jeudi
+2022-03-31</t>
+  </si>
+  <si>
+    <t>Vendredi
+2022-04-01</t>
+  </si>
+  <si>
+    <t>Samedi
+2022-04-02</t>
+  </si>
+  <si>
+    <t>dimanche
+2022-04-03</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
-    <t>F. Mayweather</t>
-  </si>
-  <si>
-    <t>C. Ronaldo</t>
-  </si>
-  <si>
-    <t>L. James</t>
-  </si>
-  <si>
-    <t>L. Messi</t>
-  </si>
-  <si>
-    <t>K. Bryant</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>T. Woods</t>
-  </si>
-  <si>
-    <t>R. Federer</t>
-  </si>
-  <si>
-    <t>P. Mickelson</t>
-  </si>
-  <si>
-    <t>R. Nadal</t>
-  </si>
-  <si>
-    <t>M. Ryan</t>
+    <t>A B</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>M. Pacquiao</t>
-  </si>
-  <si>
-    <t>Z. Ibrahimović</t>
-  </si>
-  <si>
-    <t>D. Rose</t>
-  </si>
-  <si>
-    <t>G. Bale</t>
-  </si>
-  <si>
-    <t>R. Falcao</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>M. Özil</t>
-  </si>
-  <si>
-    <t>N. Djokovic</t>
-  </si>
-  <si>
-    <t>M. Stafford</t>
-  </si>
-  <si>
-    <t>L. Hamilton</t>
-  </si>
-  <si>
-    <t>K. Durant</t>
-  </si>
-  <si>
-    <t>Semaine 14</t>
-  </si>
-  <si>
-    <t>Horaire</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Lundi
-2022-04-04</t>
-  </si>
-  <si>
-    <t>Mardi
-2022-04-05</t>
-  </si>
-  <si>
-    <t>Mercredi
-2022-04-06</t>
-  </si>
-  <si>
-    <t>Jeudi
-2022-04-07</t>
-  </si>
-  <si>
-    <t>Vendredi
-2022-04-08</t>
-  </si>
-  <si>
-    <t>Samedi
-2022-04-09</t>
-  </si>
-  <si>
-    <t>dimanche
-2022-04-10</t>
-  </si>
-  <si>
-    <t>A B</t>
-  </si>
-  <si>
     <t>C D</t>
   </si>
   <si>
-    <t>B C</t>
-  </si>
-  <si>
-    <t>Modele : repartition concentre h-pers = 1050</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> date de réf. :2022-04-08 12:12:00 
- sem : 14
- Modele : repartition concentre h-pers = 1050
- Calcul présences totales d'équipes: 30
- Calcul présences individuelles: 150.0
+    <t>Modele : repartition concentre h-pers = 900</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Calcul pr. équipes: 22
+ Calcul prés individuelles: 112.5
  Créneaux par jour: 3
  Equipes par créneau: 2
  Nombre d'équipes: 4
  Empl. par éq.: 5
- Durée quart.: 7.0
+ Durée quart.: 8.0
 </t>
   </si>
 </sst>
@@ -508,199 +436,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="20" width="20.7109375" customWidth="1"/>
-    <col min="2" max="16" width="15.7109375" customWidth="1"/>
+    <col min="1" max="15" width="23.7109375" customWidth="1"/>
+    <col min="2" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14" s="2" t="s">
-        <v>34</v>
+      <c r="A14" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="2" t="s">
-        <v>41</v>
+      <c r="A15" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refonte de la logique. dict calendrier equipes employes
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_B.xlsx
+++ b/matrice_temps/horaire_B.xlsx
@@ -81,7 +81,7 @@
  Calcul prés individuelles: 112.5
  Créneaux par jour: 3
  Equipes par créneau: 2
- Nombre d'équipes: 4
+ Nombre d'équipes: 0
  Empl. par éq.: 5
  Durée quart.: 8.0
 </t>
@@ -436,14 +436,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="15" width="23.7109375" customWidth="1"/>
-    <col min="2" max="11" width="15.7109375" customWidth="1"/>
+    <col min="1" max="17" width="23.7109375" customWidth="1"/>
+    <col min="2" max="13" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -451,48 +451,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -503,7 +481,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -514,7 +492,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -525,24 +503,46 @@
     </row>
     <row r="10" spans="1:5">
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
semi-final, check dispo rote
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_B.xlsx
+++ b/matrice_temps/horaire_B.xlsx
@@ -8,15 +8,112 @@
   </bookViews>
   <sheets>
     <sheet name="equipes" sheetId="1" r:id="rId1"/>
+    <sheet name="calendrier" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="49">
   <si>
     <t>Equipes</t>
+  </si>
+  <si>
+    <t>2022-03-28</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>F. Mayweather (35)</t>
+  </si>
+  <si>
+    <t>C. Ronaldo (100)</t>
+  </si>
+  <si>
+    <t>L. James (58)</t>
+  </si>
+  <si>
+    <t>L. Messi (61)</t>
+  </si>
+  <si>
+    <t>K. Bryant (56)</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>T. Woods (29)</t>
+  </si>
+  <si>
+    <t>R. Federer (82)</t>
+  </si>
+  <si>
+    <t>P. Mickelson (75)</t>
+  </si>
+  <si>
+    <t>R. Nadal (78)</t>
+  </si>
+  <si>
+    <t>M. Ryan (67)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>M. Pacquiao (31)</t>
+  </si>
+  <si>
+    <t>Z. Ibrahimović (99)</t>
+  </si>
+  <si>
+    <t>D. Rose (23)</t>
+  </si>
+  <si>
+    <t>G. Bale (37)</t>
+  </si>
+  <si>
+    <t>R. Falcao (77)</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>M. Özil (71)</t>
+  </si>
+  <si>
+    <t>N. Djokovic (72)</t>
+  </si>
+  <si>
+    <t>M. Stafford (48)</t>
+  </si>
+  <si>
+    <t>L. Hamilton (59)</t>
+  </si>
+  <si>
+    <t>K. Durant (55)</t>
+  </si>
+  <si>
+    <t>2022-03-29</t>
+  </si>
+  <si>
+    <t>2022-03-30</t>
+  </si>
+  <si>
+    <t>2022-03-31</t>
+  </si>
+  <si>
+    <t>F. Alonso (33)</t>
+  </si>
+  <si>
+    <t>2022-04-01</t>
+  </si>
+  <si>
+    <t>2022-04-02</t>
+  </si>
+  <si>
+    <t>2022-04-03</t>
   </si>
   <si>
     <t>Semaine 13</t>
@@ -62,13 +159,7 @@
 2022-04-03</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>A B</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>C D</t>
@@ -436,114 +527,725 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="17" width="23.7109375" customWidth="1"/>
-    <col min="2" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="36" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="2" t="s">
+      <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="2" t="s">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="2" t="s">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B25" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" s="2" t="s">
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" s="2" t="s">
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="2" t="s">
+      <c r="D35" t="s">
         <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A46:E57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="57" width="23.7109375" customWidth="1"/>
+    <col min="2" max="53" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="B47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="B48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="B49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="B50" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="B51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="B52" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="B53" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final, reste nettoyae de code.
On se rend compte que les dispos comptent 00:00 comme heure (cal)
même si elle n'est pas écrite.
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_B.xlsx
+++ b/matrice_temps/horaire_B.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="50">
   <si>
     <t>Equipes</t>
   </si>
@@ -101,13 +101,16 @@
     <t>2022-03-30</t>
   </si>
   <si>
+    <t>F. Alonso (33)</t>
+  </si>
+  <si>
     <t>2022-03-31</t>
   </si>
   <si>
-    <t>F. Alonso (33)</t>
-  </si>
-  <si>
     <t>2022-04-01</t>
+  </si>
+  <si>
+    <t>M. Singh (63)</t>
   </si>
   <si>
     <t>2022-04-02</t>
@@ -547,7 +550,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -567,7 +570,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -587,7 +590,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
@@ -607,7 +610,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
@@ -632,7 +635,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
@@ -652,7 +655,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -672,7 +675,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
@@ -692,7 +695,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
@@ -717,7 +720,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
@@ -737,72 +740,72 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
@@ -822,7 +825,7 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
@@ -842,7 +845,7 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
@@ -862,7 +865,7 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -878,7 +881,7 @@
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -887,7 +890,7 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" t="s">
@@ -897,82 +900,82 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B28" t="s">
@@ -992,7 +995,7 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B29" t="s">
@@ -1012,7 +1015,7 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B30" t="s">
@@ -1032,7 +1035,7 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B31" t="s">
@@ -1048,16 +1051,16 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B33" t="s">
@@ -1077,7 +1080,7 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B34" t="s">
@@ -1097,7 +1100,7 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B35" t="s">
@@ -1117,7 +1120,7 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B36" t="s">
@@ -1133,7 +1136,7 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1143,109 +1146,109 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A46:E57"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="57" width="23.7109375" customWidth="1"/>
-    <col min="2" max="53" width="15.7109375" customWidth="1"/>
+    <col min="1" max="13" width="23.7109375" customWidth="1"/>
+    <col min="2" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C46" t="s">
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="E46" t="s">
+      <c r="D2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="B47" s="2" t="s">
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="C47" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="B48" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="B49" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="B50" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" t="s">
-        <v>45</v>
-      </c>
-      <c r="D50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="B51" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="B52" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="B53" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="2" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>